<commit_message>
bf: update tas1 forms
</commit_message>
<xml_diff>
--- a/LF/TAS/Burkina Faso/2024/jan/bf_lf_tas1_202401_2_participant.xlsx
+++ b/LF/TAS/Burkina Faso/2024/jan/bf_lf_tas1_202401_2_participant.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bonhe\Repositories\dsa-forms\LF\TAS\Burkina Faso\2024\jan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Burkina Faso\2024\jan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6A3865-62B9-43A1-8CA8-C9C23E1335AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F77272A-FB56-478F-BF62-F6D34220B1E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="350">
   <si>
     <t>type</t>
   </si>
@@ -1072,25 +1072,34 @@
     <t>Duree_sejour_mois</t>
   </si>
   <si>
-    <t>bf_lf_tas1_202401_2_participant_2</t>
-  </si>
-  <si>
-    <t>(Jan 2024) Burkina Faso TAS FL - 2. Formulaire Enrôlement V2</t>
-  </si>
-  <si>
     <t>Cliquer suivant pour  saisir les informations sur le résultat de l’enquêté</t>
   </si>
   <si>
-    <t>1 Ancien positif</t>
-  </si>
-  <si>
     <t>2 Nouvel entrant</t>
   </si>
   <si>
-    <t>1_ancien_positif</t>
-  </si>
-  <si>
     <t>2_nouvel_entrant</t>
+  </si>
+  <si>
+    <t>bf_lf_tas1_202401_2_participant_3</t>
+  </si>
+  <si>
+    <t>(Jan 2024) Burkina Faso TAS FL - 2. Formulaire Enrôlement V3</t>
+  </si>
+  <si>
+    <t>1 Enregistré précédemment</t>
+  </si>
+  <si>
+    <t>1_enregistre_precedemment</t>
+  </si>
+  <si>
+    <t>ancien_positif</t>
+  </si>
+  <si>
+    <t>15.b. Ancien positif</t>
+  </si>
+  <si>
+    <t>${status} = '1_enregistre_precedemment'</t>
   </si>
 </sst>
 </file>
@@ -1690,11 +1699,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N52"/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1968,7 +1977,7 @@
     </row>
     <row r="13" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>78</v>
@@ -1998,7 +2007,7 @@
     </row>
     <row r="14" spans="1:14" ht="32.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>79</v>
@@ -2201,21 +2210,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
+      <c r="B25" t="s">
+        <v>347</v>
+      </c>
+      <c r="C25" t="s">
+        <v>348</v>
+      </c>
       <c r="H25" t="s">
-        <v>85</v>
+        <v>349</v>
       </c>
       <c r="J25" s="4" t="s">
         <v>10</v>
@@ -2223,19 +2229,19 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="H26" t="s">
-        <v>270</v>
+        <v>85</v>
       </c>
       <c r="J26" s="4" t="s">
         <v>10</v>
@@ -2243,70 +2249,73 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>273</v>
+        <v>169</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>274</v>
+        <v>170</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
       <c r="H27" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="H28" t="s">
+        <v>271</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>36</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>218</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H29" t="s">
         <v>85</v>
-      </c>
-      <c r="J28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" t="s">
-        <v>219</v>
-      </c>
-      <c r="H29" t="s">
-        <v>269</v>
       </c>
       <c r="J29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>167</v>
+        <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C30" t="s">
-        <v>220</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>85</v>
+        <v>219</v>
+      </c>
+      <c r="H30" t="s">
+        <v>269</v>
       </c>
       <c r="J30" t="s">
         <v>10</v>
@@ -2317,70 +2326,63 @@
         <v>167</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C31" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="J31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" t="s">
+        <v>221</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="J32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
         <v>319</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B33" s="14" t="s">
         <v>320</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C33" s="14" t="s">
         <v>241</v>
       </c>
-      <c r="D32" s="13" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>318</v>
-      </c>
-      <c r="C33" t="s">
-        <v>227</v>
-      </c>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" t="s">
-        <v>10</v>
-      </c>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
+      <c r="D33" s="13" t="s">
+        <v>340</v>
+      </c>
     </row>
     <row r="34" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>316</v>
-      </c>
-      <c r="B34" t="s">
-        <v>114</v>
+        <v>167</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>318</v>
       </c>
       <c r="C34" t="s">
-        <v>228</v>
-      </c>
-      <c r="E34" t="s">
-        <v>115</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>324</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
       <c r="I34" s="9"/>
-      <c r="J34" s="9" t="s">
+      <c r="J34" t="s">
         <v>10</v>
       </c>
       <c r="K34" s="9"/>
@@ -2388,14 +2390,17 @@
       <c r="M34" s="9"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>222</v>
+      <c r="A35" s="8" t="s">
+        <v>316</v>
       </c>
       <c r="B35" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C35" t="s">
-        <v>229</v>
+        <v>228</v>
+      </c>
+      <c r="E35" t="s">
+        <v>115</v>
       </c>
       <c r="H35" s="9" t="s">
         <v>324</v>
@@ -2410,13 +2415,13 @@
     </row>
     <row r="36" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B36" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C36" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H36" s="9" t="s">
         <v>324</v>
@@ -2431,16 +2436,16 @@
     </row>
     <row r="37" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C37" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>119</v>
+        <v>324</v>
       </c>
       <c r="I37" s="9"/>
       <c r="J37" s="9" t="s">
@@ -2452,19 +2457,16 @@
     </row>
     <row r="38" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
-        <v>9</v>
+        <v>224</v>
       </c>
       <c r="B38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C38" t="s">
-        <v>232</v>
-      </c>
-      <c r="D38" t="s">
-        <v>121</v>
+        <v>231</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="I38" s="9"/>
       <c r="J38" s="9" t="s">
@@ -2475,60 +2477,63 @@
       <c r="M38" s="9"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
-        <v>225</v>
+      <c r="A39" s="9" t="s">
+        <v>9</v>
       </c>
       <c r="B39" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C39" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D39" t="s">
-        <v>124</v>
-      </c>
-      <c r="H39" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="I39" s="10"/>
+        <v>121</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="I39" s="9"/>
       <c r="J39" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K39" s="10"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
-        <v>222</v>
+      <c r="A40" s="10" t="s">
+        <v>225</v>
       </c>
       <c r="B40" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C40" t="s">
-        <v>234</v>
-      </c>
-      <c r="F40" t="s">
-        <v>127</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="I40" s="9"/>
+        <v>233</v>
+      </c>
+      <c r="D40" t="s">
+        <v>124</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="I40" s="10"/>
       <c r="J40" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K40" s="9"/>
-      <c r="L40" s="9"/>
-      <c r="M40" s="9"/>
+      <c r="K40" s="10"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B41" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C41" t="s">
-        <v>235</v>
+        <v>234</v>
+      </c>
+      <c r="F41" t="s">
+        <v>127</v>
       </c>
       <c r="H41" s="9" t="s">
         <v>128</v>
@@ -2543,16 +2548,16 @@
     </row>
     <row r="42" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B42" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C42" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H42" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="I42" s="9"/>
       <c r="J42" s="9" t="s">
@@ -2563,59 +2568,59 @@
       <c r="M42" s="9"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
-        <v>225</v>
+      <c r="A43" s="9" t="s">
+        <v>224</v>
       </c>
       <c r="B43" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C43" t="s">
-        <v>237</v>
-      </c>
-      <c r="D43" t="s">
-        <v>133</v>
-      </c>
-      <c r="H43" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="I43" s="10"/>
+        <v>236</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="I43" s="9"/>
       <c r="J43" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K43" s="10"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
+      <c r="M43" s="9"/>
     </row>
     <row r="44" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
-        <v>226</v>
+      <c r="A44" s="10" t="s">
+        <v>225</v>
       </c>
       <c r="B44" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C44" t="s">
-        <v>238</v>
-      </c>
-      <c r="H44" s="12"/>
-      <c r="I44" s="9"/>
+        <v>237</v>
+      </c>
+      <c r="D44" t="s">
+        <v>133</v>
+      </c>
+      <c r="H44" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="I44" s="10"/>
       <c r="J44" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K44" s="9"/>
-      <c r="L44" s="9"/>
-      <c r="M44" s="9"/>
+      <c r="K44" s="10"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>9</v>
+        <v>226</v>
       </c>
       <c r="B45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C45" t="s">
-        <v>239</v>
-      </c>
-      <c r="H45" s="12" t="s">
-        <v>137</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="H45" s="12"/>
       <c r="I45" s="9"/>
       <c r="J45" s="9" t="s">
         <v>10</v>
@@ -2629,49 +2634,70 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>84</v>
+        <v>136</v>
       </c>
       <c r="C46" t="s">
-        <v>242</v>
-      </c>
-      <c r="H46" s="9" t="s">
-        <v>325</v>
+        <v>239</v>
+      </c>
+      <c r="H46" s="12" t="s">
+        <v>137</v>
       </c>
       <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
+      <c r="J46" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="K46" s="9"/>
       <c r="L46" s="9"/>
       <c r="M46" s="9"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
+    <row r="47" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B47" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47" t="s">
+        <v>242</v>
+      </c>
+      <c r="H47" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
+      <c r="M47" s="9"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B48" t="s">
         <v>61</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>98</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2683,8 +2709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3482,10 +3508,10 @@
         <v>20</v>
       </c>
       <c r="B62" t="s">
+        <v>346</v>
+      </c>
+      <c r="C62" t="s">
         <v>345</v>
-      </c>
-      <c r="C62" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -3493,10 +3519,10 @@
         <v>20</v>
       </c>
       <c r="B63" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C63" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -3973,7 +3999,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3995,10 +4021,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="B2" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="C2" t="s">
         <v>73</v>
@@ -4010,6 +4036,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008F61D857ACC8084D9287671D8B7E15F4" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b2b3977cbccd3bcf631390164057ea08">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="92042fd9-f4c9-49ed-97f1-ba485e322b1e" xmlns:ns3="744cc826-a471-4feb-879c-6424ce8a761f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5e6655229457273daeac0ec2bc1901eb" ns2:_="" ns3:_="">
     <xsd:import namespace="92042fd9-f4c9-49ed-97f1-ba485e322b1e"/>
@@ -4238,16 +4273,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AA70DE9-52EB-4A74-A92B-6BC33DECE403}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7691146D-9A17-4B60-A330-159941DFBC25}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4264,12 +4298,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6AA70DE9-52EB-4A74-A92B-6BC33DECE403}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>